<commit_message>
update Excel tables in Quadratics and Non Convex
</commit_message>
<xml_diff>
--- a/experiment/results/No Convexos/Fuertemente-Estacionarios.xlsx
+++ b/experiment/results/No Convexos/Fuertemente-Estacionarios.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>Nombre Problema</t>
   </si>
@@ -56,6 +56,12 @@
     <t>(0.8,1.85)</t>
   </si>
   <si>
+    <t>(3.45,1.85)</t>
+  </si>
+  <si>
+    <t>37.05</t>
+  </si>
+  <si>
     <t>MitsosBarton2006Ex313</t>
   </si>
   <si>
@@ -65,16 +71,40 @@
     <t xml:space="preserve">   - 2.15</t>
   </si>
   <si>
+    <t xml:space="preserve"> -2.16</t>
+  </si>
+  <si>
     <t>MitsosBarton2006Ex314</t>
   </si>
   <si>
     <t>(2.1,3.3)</t>
   </si>
   <si>
+    <t>14.31</t>
+  </si>
+  <si>
+    <t>(2.1,-1.45)</t>
+  </si>
+  <si>
+    <t>5.52</t>
+  </si>
+  <si>
     <t>MitsosBarton2006Ex323</t>
   </si>
   <si>
+    <t>(2.89,0.3)</t>
+  </si>
+  <si>
+    <t>8.35</t>
+  </si>
+  <si>
     <t>MorganPatrone2006a</t>
+  </si>
+  <si>
+    <t>(4.5,2.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -7.3</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1043,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -1022,7 +1052,7 @@
     <col min="2" max="2" width="28.2727272727273" customWidth="1"/>
     <col min="3" max="3" width="44.2727272727273" customWidth="1"/>
     <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
-    <col min="5" max="5" width="55.6363636363636" customWidth="1"/>
+    <col min="5" max="5" width="24.4545454545455" customWidth="1"/>
     <col min="6" max="6" width="45.0909090909091" customWidth="1"/>
     <col min="7" max="7" width="12.4545454545455" customWidth="1"/>
   </cols>
@@ -1050,7 +1080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1063,8 +1093,14 @@
       <c r="D3" s="1">
         <v>34939</v>
       </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1077,84 +1113,171 @@
       <c r="D4" s="1">
         <v>34939</v>
       </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>9</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
       </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>